<commit_message>
AutoCommit_25 февраля 2024 г. 16:11:46_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -736,7 +736,9 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -778,7 +780,9 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -836,7 +840,9 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_29 февраля 2024 г. 15:24:34_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,9 @@
       <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_7 марта 2024 г. 12:26:06_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,9 @@
       <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_7 марта 2024 г. 12:44:58_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,9 @@
       <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_21 марта 2024 г. 13:54:09_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -563,8 +563,12 @@
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -682,10 +686,16 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -800,9 +810,15 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -865,9 +881,15 @@
       <c r="C25" s="2">
         <v>5</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
@@ -881,9 +903,15 @@
       <c r="C26" s="2">
         <v>5</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -897,8 +925,12 @@
       <c r="C27" s="2">
         <v>5</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_21 марта 2024 г. 13:54:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -850,8 +850,12 @@
       <c r="D23" s="2">
         <v>5</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_21 марта 2024 г. 15:27:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -672,10 +672,18 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_4 апреля 2024 г. 10:07:24_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -805,9 +805,15 @@
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 16:52:00_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -145,12 +145,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -189,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -201,6 +207,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,13 +516,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -523,12 +532,12 @@
     <col min="3" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -549,7 +558,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -557,23 +566,25 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="J4">
@@ -583,24 +594,27 @@
       <c r="K4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
         <v>5</v>
       </c>
       <c r="G5" s="2"/>
@@ -612,18 +626,29 @@
       <c r="K5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="J6">
@@ -633,20 +658,29 @@
       <c r="K6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
       <c r="G7" s="2">
         <v>5</v>
       </c>
@@ -658,24 +692,27 @@
       <c r="K7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
         <v>5</v>
       </c>
       <c r="G8" s="2"/>
@@ -687,18 +724,29 @@
       <c r="K8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="J9">
@@ -708,18 +756,29 @@
       <c r="K9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="J10">
@@ -729,24 +788,27 @@
       <c r="K10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5">
         <v>5</v>
       </c>
       <c r="G11" s="2"/>
@@ -758,24 +820,27 @@
       <c r="K11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
         <v>5</v>
       </c>
       <c r="G12" s="2"/>
@@ -787,22 +852,27 @@
       <c r="K12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
         <v>5</v>
       </c>
       <c r="G13" s="2"/>
@@ -814,20 +884,29 @@
       <c r="K13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="J14">
@@ -837,18 +916,29 @@
       <c r="K14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="J15">
@@ -858,18 +948,29 @@
       <c r="K15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="J16">
@@ -879,22 +980,27 @@
       <c r="K16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2">
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
         <v>5</v>
       </c>
       <c r="G17" s="2"/>
@@ -906,24 +1012,29 @@
       <c r="K17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>5</v>
-      </c>
-      <c r="F18" s="2"/>
+      <c r="C18" s="5">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="J18">
@@ -933,18 +1044,29 @@
       <c r="K18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="J19">
@@ -954,24 +1076,27 @@
       <c r="K19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
         <v>5</v>
       </c>
       <c r="G20" s="2"/>
@@ -983,24 +1108,29 @@
       <c r="K20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5">
+        <v>5</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="J21">
@@ -1010,24 +1140,27 @@
       <c r="K21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5">
+        <v>5</v>
+      </c>
+      <c r="F22" s="5">
         <v>5</v>
       </c>
       <c r="G22" s="2"/>
@@ -1039,24 +1172,27 @@
       <c r="K22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5">
+        <v>5</v>
+      </c>
+      <c r="F23" s="5">
         <v>5</v>
       </c>
       <c r="G23" s="2"/>
@@ -1068,20 +1204,27 @@
       <c r="K23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2">
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
         <v>5</v>
       </c>
       <c r="G24" s="2"/>
@@ -1093,24 +1236,27 @@
       <c r="K24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5">
+        <v>5</v>
+      </c>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
+      <c r="F25" s="5">
         <v>5</v>
       </c>
       <c r="G25" s="2"/>
@@ -1123,23 +1269,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="C26" s="5">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5">
+        <v>5</v>
+      </c>
+      <c r="F26" s="5">
         <v>5</v>
       </c>
       <c r="G26" s="2"/>
@@ -1152,23 +1298,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2"/>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="J27">
@@ -1179,17 +1327,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="J28">
@@ -1200,17 +1356,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="J29">
@@ -1221,21 +1385,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2"/>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>5</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="J30">
@@ -1246,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_19 апреля 2024 г. 8:30:47_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -519,10 +519,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -582,14 +582,16 @@
       <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="J4">
         <f>SUM(C4:H4)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K4">
         <v>4</v>
@@ -617,11 +619,15 @@
       <c r="F5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
       <c r="J5">
         <f t="shared" ref="J5:J30" si="0">SUM(C5:H5)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -735,23 +741,23 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0</v>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -869,17 +875,19 @@
       <c r="D13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
+      <c r="E13" s="2">
+        <v>5</v>
       </c>
       <c r="F13" s="5">
         <v>5</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K13">
         <v>4</v>
@@ -1055,23 +1063,23 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0</v>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K19">
         <v>3</v>
@@ -1288,11 +1296,15 @@
       <c r="F26" s="5">
         <v>5</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="G26" s="2">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2">
+        <v>5</v>
+      </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="K26">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_26 апреля 2024 г. 12:19:03_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -522,7 +522,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -643,23 +643,27 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K6">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_23 мая 2024 г. 15:31:08_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ИСИП-322: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -120,10 +120,13 @@
     <t>ДЗ_5</t>
   </si>
   <si>
-    <t>Сумм</t>
-  </si>
-  <si>
     <t>Лаб</t>
+  </si>
+  <si>
+    <t>ДЗ_6</t>
+  </si>
+  <si>
+    <t>ДЗ_7</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,15 +192,6 @@
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
@@ -209,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -220,16 +214,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -539,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -557,7 +548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -573,15 +564,17 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -596,13 +589,13 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
         <v>5</v>
       </c>
       <c r="F4" s="2">
@@ -612,13 +605,6 @@
         <v>5</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="J4">
-        <f>SUM(C4:H4)</f>
-        <v>25</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
       <c r="L4">
         <v>0</v>
       </c>
@@ -630,16 +616,16 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
         <v>5</v>
       </c>
       <c r="G5" s="2">
@@ -647,13 +633,6 @@
       </c>
       <c r="H5" s="2">
         <v>5</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J30" si="0">SUM(C5:H5)</f>
-        <v>30</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -684,13 +663,6 @@
       <c r="H6" s="2">
         <v>5</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
       <c r="L6">
         <v>0</v>
       </c>
@@ -702,29 +674,22 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5">
-        <v>2</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
         <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
       <c r="L7">
         <v>0</v>
       </c>
@@ -736,29 +701,22 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5</v>
-      </c>
-      <c r="E8" s="5">
-        <v>5</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4">
         <v>5</v>
       </c>
       <c r="G8" s="2">
         <v>5</v>
       </c>
       <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K8">
         <v>5</v>
       </c>
       <c r="L8">
@@ -786,13 +744,6 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
       <c r="L9">
         <v>0</v>
       </c>
@@ -804,27 +755,20 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
-        <v>2</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4">
         <v>2</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
       <c r="L10">
         <v>0</v>
       </c>
@@ -836,16 +780,16 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
-        <v>5</v>
-      </c>
-      <c r="D11" s="5">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5">
-        <v>5</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
         <v>5</v>
       </c>
       <c r="G11" s="2">
@@ -855,10 +799,6 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K11">
         <v>5</v>
       </c>
       <c r="L11">
@@ -872,27 +812,20 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5">
-        <v>5</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
         <v>5</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
       <c r="L12">
         <v>0</v>
       </c>
@@ -904,29 +837,22 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4">
         <v>5</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>5</v>
       </c>
       <c r="G13" s="2">
         <v>5</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="K13">
-        <v>4</v>
-      </c>
       <c r="L13">
         <v>0</v>
       </c>
@@ -938,27 +864,20 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5">
-        <v>5</v>
-      </c>
-      <c r="D14" s="5">
-        <v>2</v>
-      </c>
-      <c r="E14" s="5">
-        <v>2</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4">
         <v>2</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
       <c r="L14">
         <v>0</v>
       </c>
@@ -970,27 +889,20 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
-        <v>2</v>
-      </c>
-      <c r="D15" s="5">
-        <v>2</v>
-      </c>
-      <c r="E15" s="5">
-        <v>2</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4">
         <v>2</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
       <c r="L15">
         <v>0</v>
       </c>
@@ -1016,13 +928,6 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K16">
-        <v>3</v>
-      </c>
       <c r="L16">
         <v>0</v>
       </c>
@@ -1034,27 +939,20 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5">
-        <v>2</v>
-      </c>
-      <c r="F17" s="5">
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
         <v>5</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="K17">
-        <v>4</v>
-      </c>
       <c r="L17">
         <v>0</v>
       </c>
@@ -1066,27 +964,20 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5">
-        <v>5</v>
-      </c>
-      <c r="D18" s="5">
-        <v>5</v>
-      </c>
-      <c r="E18" s="5">
-        <v>5</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4">
         <v>2</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="K18">
-        <v>4</v>
-      </c>
       <c r="L18">
         <v>0</v>
       </c>
@@ -1112,15 +1003,8 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="7">
-        <v>5</v>
-      </c>
-      <c r="J19">
-        <f>SUM(C19:I19)</f>
-        <v>25</v>
-      </c>
-      <c r="K19">
-        <v>3</v>
+      <c r="I19" s="6">
+        <v>5</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1133,29 +1017,22 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5">
-        <v>5</v>
-      </c>
-      <c r="D20" s="5">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5">
-        <v>5</v>
-      </c>
-      <c r="F20" s="5">
+      <c r="C20" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4">
         <v>5</v>
       </c>
       <c r="G20" s="2">
         <v>5</v>
       </c>
       <c r="H20" s="2">
-        <v>5</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K20">
         <v>5</v>
       </c>
       <c r="L20">
@@ -1169,13 +1046,13 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5">
-        <v>5</v>
-      </c>
-      <c r="D21" s="5">
-        <v>5</v>
-      </c>
-      <c r="E21" s="5">
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
         <v>5</v>
       </c>
       <c r="F21" s="2">
@@ -1186,13 +1063,6 @@
       </c>
       <c r="H21" s="2">
         <v>5</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K21">
-        <v>4</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1205,27 +1075,20 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5">
-        <v>5</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4">
         <v>5</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K22">
-        <v>5</v>
-      </c>
       <c r="L22">
         <v>0</v>
       </c>
@@ -1237,29 +1100,22 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="5">
-        <v>5</v>
-      </c>
-      <c r="D23" s="5">
-        <v>5</v>
-      </c>
-      <c r="E23" s="5">
-        <v>5</v>
-      </c>
-      <c r="F23" s="5">
+      <c r="C23" s="4">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
+      <c r="E23" s="4">
+        <v>5</v>
+      </c>
+      <c r="F23" s="4">
         <v>5</v>
       </c>
       <c r="G23" s="2">
         <v>5</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="K23">
-        <v>5</v>
-      </c>
       <c r="L23">
         <v>0</v>
       </c>
@@ -1271,27 +1127,20 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="5">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5">
-        <v>2</v>
-      </c>
-      <c r="E24" s="5">
-        <v>2</v>
-      </c>
-      <c r="F24" s="5">
+      <c r="C24" s="4">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4">
         <v>5</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="K24">
-        <v>4</v>
-      </c>
       <c r="L24">
         <v>0</v>
       </c>
@@ -1303,27 +1152,20 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="5">
-        <v>5</v>
-      </c>
-      <c r="D25" s="5">
-        <v>5</v>
-      </c>
-      <c r="E25" s="5">
-        <v>5</v>
-      </c>
-      <c r="F25" s="5">
+      <c r="C25" s="4">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5</v>
+      </c>
+      <c r="E25" s="4">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4">
         <v>5</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="K25">
-        <v>5</v>
-      </c>
     </row>
     <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -1332,29 +1174,22 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="5">
-        <v>5</v>
-      </c>
-      <c r="D26" s="5">
-        <v>5</v>
-      </c>
-      <c r="E26" s="5">
-        <v>5</v>
-      </c>
-      <c r="F26" s="5">
+      <c r="C26" s="4">
+        <v>5</v>
+      </c>
+      <c r="D26" s="4">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4">
         <v>5</v>
       </c>
       <c r="G26" s="2">
         <v>5</v>
       </c>
       <c r="H26" s="2">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K26">
         <v>5</v>
       </c>
     </row>
@@ -1365,13 +1200,13 @@
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5">
-        <v>5</v>
-      </c>
-      <c r="D27" s="5">
-        <v>5</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="C27" s="4">
+        <v>5</v>
+      </c>
+      <c r="D27" s="4">
+        <v>5</v>
+      </c>
+      <c r="E27" s="4">
         <v>5</v>
       </c>
       <c r="F27" s="2">
@@ -1382,13 +1217,6 @@
       </c>
       <c r="H27" s="2">
         <v>5</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="K27">
-        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,21 +1232,14 @@
       <c r="D28" s="2">
         <v>5</v>
       </c>
-      <c r="E28" s="5">
-        <v>2</v>
-      </c>
-      <c r="F28" s="5">
+      <c r="E28" s="4">
+        <v>2</v>
+      </c>
+      <c r="F28" s="4">
         <v>2</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="K28">
-        <v>3</v>
-      </c>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1427,27 +1248,20 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="5">
-        <v>2</v>
-      </c>
-      <c r="D29" s="5">
-        <v>2</v>
-      </c>
-      <c r="E29" s="5">
-        <v>2</v>
-      </c>
-      <c r="F29" s="5">
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2</v>
+      </c>
+      <c r="F29" s="4">
         <v>2</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="J29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K29">
-        <v>3</v>
-      </c>
     </row>
     <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1456,27 +1270,20 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="5">
-        <v>5</v>
-      </c>
-      <c r="D30" s="5">
-        <v>2</v>
-      </c>
-      <c r="E30" s="5">
-        <v>5</v>
-      </c>
-      <c r="F30" s="5">
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+      <c r="D30" s="4">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4">
         <v>2</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="J30">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="K30">
-        <v>4</v>
-      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 10:11:01_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -891,19 +891,21 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="L15">
         <v>0</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 14:14:32_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -949,13 +949,15 @@
       <c r="D17" s="4">
         <v>5</v>
       </c>
-      <c r="E17" s="4">
-        <v>2</v>
+      <c r="E17" s="2">
+        <v>5</v>
       </c>
       <c r="F17" s="4">
         <v>5</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2">
+        <v>5</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="L17">
         <v>0</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 14:40:04_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -609,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -634,11 +634,14 @@
       <c r="H5" s="2">
         <v>5</v>
       </c>
+      <c r="J5" s="2">
+        <v>5</v>
+      </c>
       <c r="L5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1180,7 +1183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1205,8 +1208,11 @@
       <c r="H26" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1308,7 +1314,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="J4:J30">
+  <conditionalFormatting sqref="J27:J30 J4 J6:J25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 15:00:18_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,9 @@
       <c r="G17" s="2">
         <v>5</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
       <c r="L17">
         <v>0</v>
       </c>
@@ -1142,16 +1144,18 @@
       <c r="C24" s="4">
         <v>5</v>
       </c>
-      <c r="D24" s="4">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4">
-        <v>2</v>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
       </c>
       <c r="F24" s="4">
         <v>5</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2">
+        <v>5</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="L24">
         <v>0</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 15:03:24_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,9 @@
       <c r="G13" s="2">
         <v>5</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
       <c r="L13">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 15:25:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -634,6 +634,9 @@
       <c r="H5" s="2">
         <v>5</v>
       </c>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
       <c r="J5" s="2">
         <v>5</v>
       </c>
@@ -670,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -692,12 +695,17 @@
       <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
       <c r="L7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -722,11 +730,17 @@
       <c r="H8" s="2">
         <v>5</v>
       </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
       <c r="L8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -751,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -776,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -801,6 +815,9 @@
       <c r="H11" s="2">
         <v>5</v>
       </c>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
       <c r="J11">
         <v>5</v>
       </c>
@@ -808,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -833,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -858,11 +875,17 @@
       <c r="H13" s="2">
         <v>5</v>
       </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
       <c r="L13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1212,6 +1235,9 @@
         <v>5</v>
       </c>
       <c r="H26" s="2">
+        <v>5</v>
+      </c>
+      <c r="I26" s="2">
         <v>5</v>
       </c>
       <c r="J26" s="2">
@@ -1320,7 +1346,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="J27:J30 J4 J6:J25">
+  <conditionalFormatting sqref="J27:J30 J4 J6 J9:J12 J14:J25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_7 июня 2024 г. 9:47:22_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -221,6 +221,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,10 +533,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1071,6 +1074,12 @@
       <c r="H20" s="2">
         <v>5</v>
       </c>
+      <c r="I20" s="7">
+        <v>5</v>
+      </c>
+      <c r="J20" s="7">
+        <v>5</v>
+      </c>
       <c r="L20">
         <v>0</v>
       </c>
@@ -1267,6 +1276,12 @@
         <v>5</v>
       </c>
       <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="I27" s="6">
+        <v>5</v>
+      </c>
+      <c r="J27" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 9:34:20_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -165,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,11 +199,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -224,6 +233,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,10 +545,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -937,7 +949,12 @@
       <c r="G15" s="2">
         <v>5</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="8">
+        <v>5</v>
+      </c>
       <c r="L15">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 11:18:28_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -545,10 +545,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1124,6 +1124,12 @@
         <v>5</v>
       </c>
       <c r="H21" s="2">
+        <v>5</v>
+      </c>
+      <c r="I21" s="6">
+        <v>5</v>
+      </c>
+      <c r="J21" s="8">
         <v>5</v>
       </c>
       <c r="L21">

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:01:57_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -241,6 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,10 +549,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -935,7 +936,15 @@
       <c r="G14" s="2">
         <v>5</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="7">
+        <v>5</v>
+      </c>
+      <c r="J14" s="10">
+        <v>5</v>
+      </c>
       <c r="L14">
         <v>0</v>
       </c>
@@ -963,6 +972,9 @@
         <v>5</v>
       </c>
       <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="I15" s="6">
         <v>5</v>
       </c>
       <c r="J15" s="8">

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:07:38_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -549,10 +549,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -873,8 +873,18 @@
       <c r="F12" s="4">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="8">
+        <v>5</v>
+      </c>
+      <c r="J12" s="9">
+        <v>5</v>
+      </c>
       <c r="L12">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:18:17_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -549,10 +549,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1042,6 +1042,12 @@
         <v>5</v>
       </c>
       <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" s="8">
+        <v>5</v>
+      </c>
+      <c r="J17" s="9">
         <v>5</v>
       </c>
       <c r="L17">

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:25:51_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -548,11 +548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -623,9 +623,18 @@
       <c r="G4" s="2">
         <v>5</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>5</v>
+      </c>
+      <c r="J4" s="8">
+        <v>5</v>
+      </c>
       <c r="L4">
-        <v>0</v>
+        <f>SUM(C4:J4)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -660,7 +669,8 @@
         <v>5</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <f t="shared" ref="L5:L30" si="0">SUM(C5:J5)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -689,7 +699,8 @@
         <v>5</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -721,7 +732,8 @@
         <v>5</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -756,7 +768,8 @@
         <v>5</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -791,7 +804,8 @@
         <v>5</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -816,7 +830,8 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="L10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -851,7 +866,8 @@
         <v>5</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -886,7 +902,8 @@
         <v>5</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -921,7 +938,8 @@
         <v>5</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -956,7 +974,8 @@
         <v>5</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,7 +1010,8 @@
         <v>5</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1016,7 +1036,8 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="L16">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,7 +1072,8 @@
         <v>5</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,7 +1098,8 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="L18">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1111,7 +1134,8 @@
         <v>5</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,7 +1170,8 @@
         <v>5</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1181,7 +1206,8 @@
         <v>5</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1209,7 +1235,8 @@
         <v>5</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1236,7 +1263,8 @@
       </c>
       <c r="H23" s="2"/>
       <c r="L23">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1265,7 +1293,8 @@
         <v>5</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1299,6 +1328,10 @@
       <c r="J25" s="7">
         <v>5</v>
       </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -1331,6 +1364,10 @@
       <c r="J26" s="2">
         <v>5</v>
       </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1363,6 +1400,10 @@
       <c r="J27" s="6">
         <v>5</v>
       </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1395,6 +1436,10 @@
       <c r="J28" s="6">
         <v>5</v>
       </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1417,6 +1462,10 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1439,6 +1488,10 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
@@ -1451,6 +1504,18 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="J27:J30 J4 J6 J9:J12 J14:J25">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:44:05_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -549,10 +549,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1092,17 +1092,24 @@
       <c r="E18" s="4">
         <v>5</v>
       </c>
-      <c r="F18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1455,7 +1462,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1481,7 +1488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1491,23 +1498,33 @@
       <c r="C30" s="4">
         <v>5</v>
       </c>
-      <c r="D30" s="4">
-        <v>2</v>
+      <c r="D30" s="2">
+        <v>5</v>
       </c>
       <c r="E30" s="4">
         <v>5</v>
       </c>
-      <c r="F30" s="4">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>5</v>
+      </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1517,7 +1534,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="J27:J30 J4 J6 J9:J12 J14:J25">
+  <conditionalFormatting sqref="J27:J29 J4 J6 J9:J12 J14:J17 J19:J25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 12:35:12_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -549,10 +549,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1033,11 +1033,21 @@
       <c r="F16" s="2">
         <v>5</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5</v>
+      </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 13:13:09_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -548,11 +548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1111,12 +1111,15 @@
       <c r="H18" s="2">
         <v>5</v>
       </c>
+      <c r="I18" s="8">
+        <v>5</v>
+      </c>
       <c r="J18" s="2">
         <v>5</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 8:41:45_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-322_ТерВер.xlsx
+++ b/_2ИСИП-322_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>2ИСИП-322: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>ДЗ_7</t>
+  </si>
+  <si>
+    <t>сумма</t>
   </si>
 </sst>
 </file>
@@ -160,7 +163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,36 +215,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -546,28 +544,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="41.6328125" customWidth="1"/>
-    <col min="3" max="8" width="5.1796875" customWidth="1"/>
+    <col min="3" max="10" width="4.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -589,11 +587,11 @@
       <c r="I2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -612,15 +610,18 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="3"/>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -636,16 +637,16 @@
       <c r="E4" s="4">
         <v>5</v>
       </c>
-      <c r="F4" s="2">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2">
-        <v>5</v>
-      </c>
-      <c r="I4" s="8">
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5">
         <v>5</v>
       </c>
       <c r="J4" s="6">
@@ -655,8 +656,11 @@
         <f t="shared" ref="L4:L30" si="0">SUM(C4:J4)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -675,60 +679,66 @@
       <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
-        <v>5</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4">
         <v>5</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
         <v>5</v>
       </c>
       <c r="I6" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="M6" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -738,33 +748,36 @@
       <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5</v>
-      </c>
-      <c r="I7" s="2">
-        <v>5</v>
-      </c>
-      <c r="J7" s="8">
-        <v>2</v>
+      <c r="D7" s="7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="M7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -783,49 +796,52 @@
       <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="G8" s="4">
+        <v>5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5</v>
+      </c>
+      <c r="J8" s="4">
         <v>5</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="8">
         <v>5</v>
       </c>
       <c r="J9" s="6">
@@ -835,8 +851,11 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -844,35 +863,38 @@
         <v>7</v>
       </c>
       <c r="C10" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2</v>
-      </c>
-      <c r="I10" s="9">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
       </c>
       <c r="J10" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -891,24 +913,27 @@
       <c r="F11" s="4">
         <v>5</v>
       </c>
-      <c r="G11" s="2">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="G11" s="4">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="4">
         <v>5</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -927,24 +952,27 @@
       <c r="F12" s="4">
         <v>5</v>
       </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="9">
-        <v>5</v>
-      </c>
-      <c r="J12" s="8">
+      <c r="G12" s="4">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5</v>
+      </c>
+      <c r="I12" s="8">
+        <v>5</v>
+      </c>
+      <c r="J12" s="5">
         <v>5</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -957,30 +985,33 @@
       <c r="D13" s="4">
         <v>5</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>5</v>
       </c>
       <c r="F13" s="4">
         <v>5</v>
       </c>
-      <c r="G13" s="2">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2">
-        <v>5</v>
-      </c>
-      <c r="I13" s="2">
-        <v>5</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>5</v>
+      </c>
+      <c r="I13" s="4">
+        <v>5</v>
+      </c>
+      <c r="J13" s="4">
         <v>5</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -999,49 +1030,52 @@
       <c r="F14" s="4">
         <v>5</v>
       </c>
-      <c r="G14" s="2">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2">
-        <v>5</v>
-      </c>
-      <c r="I14" s="10">
-        <v>5</v>
-      </c>
-      <c r="J14" s="7">
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="I14" s="9">
+        <v>5</v>
+      </c>
+      <c r="J14" s="6">
         <v>5</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
-        <v>5</v>
-      </c>
-      <c r="G15" s="2">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2">
-        <v>5</v>
-      </c>
-      <c r="I15" s="8">
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+      <c r="G15" s="4">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5</v>
+      </c>
+      <c r="I15" s="5">
         <v>5</v>
       </c>
       <c r="J15" s="6">
@@ -1051,44 +1085,50 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2">
-        <v>5</v>
-      </c>
-      <c r="H16" s="2">
-        <v>5</v>
-      </c>
-      <c r="I16" s="8">
-        <v>5</v>
-      </c>
-      <c r="J16" s="8">
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="5">
+        <v>5</v>
+      </c>
+      <c r="J16" s="5">
         <v>5</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1101,30 +1141,33 @@
       <c r="D17" s="4">
         <v>5</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="4">
         <v>5</v>
       </c>
       <c r="F17" s="4">
         <v>5</v>
       </c>
-      <c r="G17" s="2">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2">
-        <v>5</v>
-      </c>
-      <c r="I17" s="9">
-        <v>5</v>
-      </c>
-      <c r="J17" s="8">
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5</v>
+      </c>
+      <c r="I17" s="8">
+        <v>5</v>
+      </c>
+      <c r="J17" s="5">
         <v>5</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1140,49 +1183,52 @@
       <c r="E18" s="4">
         <v>5</v>
       </c>
-      <c r="F18" s="2">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2">
-        <v>5</v>
-      </c>
-      <c r="J18" s="8">
+      <c r="F18" s="4">
+        <v>5</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5</v>
+      </c>
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5</v>
+      </c>
+      <c r="J18" s="5">
         <v>5</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4">
+        <v>5</v>
+      </c>
+      <c r="G19" s="4">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4">
         <v>5</v>
       </c>
       <c r="I19" s="6">
@@ -1195,8 +1241,11 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1215,24 +1264,27 @@
       <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="G20" s="2">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2">
-        <v>5</v>
-      </c>
-      <c r="I20" s="7">
-        <v>5</v>
-      </c>
-      <c r="J20" s="7">
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>5</v>
+      </c>
+      <c r="I20" s="6">
+        <v>5</v>
+      </c>
+      <c r="J20" s="6">
         <v>5</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1248,16 +1300,16 @@
       <c r="E21" s="4">
         <v>5</v>
       </c>
-      <c r="F21" s="2">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2">
-        <v>5</v>
-      </c>
-      <c r="I21" s="8">
+      <c r="F21" s="4">
+        <v>5</v>
+      </c>
+      <c r="G21" s="4">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4">
+        <v>5</v>
+      </c>
+      <c r="I21" s="5">
         <v>5</v>
       </c>
       <c r="J21" s="6">
@@ -1267,8 +1319,11 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1287,13 +1342,13 @@
       <c r="F22" s="4">
         <v>5</v>
       </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2">
-        <v>5</v>
-      </c>
-      <c r="I22" s="9">
+      <c r="G22" s="4">
+        <v>5</v>
+      </c>
+      <c r="H22" s="4">
+        <v>5</v>
+      </c>
+      <c r="I22" s="8">
         <v>5</v>
       </c>
       <c r="J22" s="6">
@@ -1303,8 +1358,11 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1323,24 +1381,27 @@
       <c r="F23" s="4">
         <v>5</v>
       </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2">
-        <v>5</v>
-      </c>
-      <c r="I23">
-        <v>5</v>
-      </c>
-      <c r="J23" s="8">
+      <c r="G23" s="4">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+      <c r="I23" s="7">
+        <v>5</v>
+      </c>
+      <c r="J23" s="5">
         <v>5</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1350,33 +1411,36 @@
       <c r="C24" s="4">
         <v>5</v>
       </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="4">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4">
         <v>5</v>
       </c>
       <c r="F24" s="4">
         <v>5</v>
       </c>
-      <c r="G24" s="2">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="8">
-        <v>5</v>
-      </c>
-      <c r="J24" s="8">
+      <c r="G24" s="4">
+        <v>5</v>
+      </c>
+      <c r="H24" s="4">
+        <v>5</v>
+      </c>
+      <c r="I24" s="5">
+        <v>5</v>
+      </c>
+      <c r="J24" s="5">
         <v>5</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1395,24 +1459,27 @@
       <c r="F25" s="4">
         <v>5</v>
       </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>5</v>
-      </c>
-      <c r="I25" s="7">
-        <v>5</v>
-      </c>
-      <c r="J25" s="7">
+      <c r="G25" s="4">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4">
+        <v>5</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6">
         <v>5</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1431,24 +1498,27 @@
       <c r="F26" s="4">
         <v>5</v>
       </c>
-      <c r="G26" s="2">
-        <v>5</v>
-      </c>
-      <c r="H26" s="2">
-        <v>5</v>
-      </c>
-      <c r="I26" s="2">
-        <v>5</v>
-      </c>
-      <c r="J26" s="2">
+      <c r="G26" s="4">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4">
+        <v>5</v>
+      </c>
+      <c r="J26" s="4">
         <v>5</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1464,13 +1534,13 @@
       <c r="E27" s="4">
         <v>5</v>
       </c>
-      <c r="F27" s="2">
-        <v>5</v>
-      </c>
-      <c r="G27" s="2">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2">
+      <c r="F27" s="4">
+        <v>5</v>
+      </c>
+      <c r="G27" s="4">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
         <v>5</v>
       </c>
       <c r="I27" s="6">
@@ -1483,30 +1553,33 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2">
-        <v>5</v>
-      </c>
-      <c r="G28" s="2">
-        <v>5</v>
-      </c>
-      <c r="H28" s="2">
+      <c r="C28" s="4">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>5</v>
+      </c>
+      <c r="F28" s="4">
+        <v>5</v>
+      </c>
+      <c r="G28" s="4">
+        <v>5</v>
+      </c>
+      <c r="H28" s="4">
         <v>5</v>
       </c>
       <c r="I28" s="6">
@@ -1519,8 +1592,11 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1528,35 +1604,38 @@
         <v>26</v>
       </c>
       <c r="C29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>2</v>
-      </c>
-      <c r="G29" s="2">
-        <v>2</v>
-      </c>
-      <c r="H29" s="2">
-        <v>2</v>
-      </c>
-      <c r="I29" s="8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
       </c>
       <c r="J29" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1566,43 +1645,46 @@
       <c r="C30" s="4">
         <v>5</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
         <v>5</v>
       </c>
       <c r="E30" s="4">
         <v>5</v>
       </c>
-      <c r="F30" s="2">
-        <v>5</v>
-      </c>
-      <c r="G30" s="2">
-        <v>5</v>
-      </c>
-      <c r="H30" s="2">
-        <v>5</v>
-      </c>
-      <c r="I30" s="2">
-        <v>5</v>
-      </c>
-      <c r="J30" s="2">
+      <c r="F30" s="4">
+        <v>5</v>
+      </c>
+      <c r="G30" s="4">
+        <v>5</v>
+      </c>
+      <c r="H30" s="4">
+        <v>5</v>
+      </c>
+      <c r="I30" s="4">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4">
         <v>5</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="M30" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="I27:I29 I4 I6 I9:I12 I14:I17 I19:I25">
+  <conditionalFormatting sqref="C4:J30 M12:M30 M4:M10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>